<commit_message>
data pull numero uno
</commit_message>
<xml_diff>
--- a/finalData/Productfinal.xlsx
+++ b/finalData/Productfinal.xlsx
@@ -3,21 +3,21 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="9660" windowWidth="16092" xWindow="240" yWindow="12"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="9660" windowWidth="16095" xWindow="240" yWindow="15"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Sheet 2" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -34,11 +34,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <name val="Calibri"/>
-      <b val="1"/>
-      <sz val="11"/>
-    </font>
-    <font>
       <b val="1"/>
     </font>
   </fonts>
@@ -50,27 +45,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -99,15 +79,12 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf applyAlignment="1" borderId="2" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf applyAlignment="1" borderId="3" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -407,70 +384,71 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K46"/>
+  <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
-  <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" width="18.109375"/>
-    <col bestFit="1" customWidth="1" max="2" min="2" width="125.44140625"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>Time</t>
         </is>
       </c>
-      <c r="B1" s="3" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>Tweet</t>
         </is>
       </c>
-      <c r="C1" s="3" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>Favorites</t>
         </is>
       </c>
-      <c r="D1" s="3" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>Retweets</t>
         </is>
       </c>
-      <c r="E1" s="3" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>Sentiment</t>
         </is>
       </c>
-      <c r="F1" s="3" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>Material</t>
         </is>
       </c>
-      <c r="G1" s="3" t="inlineStr">
+      <c r="G1" s="2" t="inlineStr">
         <is>
           <t>Category1</t>
         </is>
       </c>
-      <c r="H1" s="3" t="inlineStr">
+      <c r="H1" s="2" t="inlineStr">
         <is>
           <t>Category2</t>
         </is>
       </c>
-      <c r="I1" s="3" t="inlineStr">
+      <c r="I1" s="2" t="inlineStr">
         <is>
           <t>Category3</t>
         </is>
       </c>
-      <c r="J1" s="3" t="inlineStr">
+      <c r="J1" s="2" t="inlineStr">
         <is>
           <t>keyPhrases</t>
         </is>
       </c>
-      <c r="K1" s="3" t="inlineStr">
+      <c r="K1" s="2" t="inlineStr">
+        <is>
+          <t>News</t>
+        </is>
+      </c>
+      <c r="L1" s="2" t="inlineStr">
         <is>
           <t>Irrelevent</t>
         </is>
@@ -479,22 +457,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2019-06-27 20:20:48</t>
+          <t>2019-06-24 18:40:26</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>RT @LittleJohn_MD: My Son brought me home a Japanese Codd fruit drink bottle. Never knew they still made the old Codd bottle. Fascinating w</t>
+          <t>Reusing packaging whenever possible is one simple way we can all make a difference. We make it especially easy with https://t.co/8na8uyMBzh</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0.8085362911224365</v>
+        <v>0.9514744281768799</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -510,32 +488,35 @@
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr">
         <is>
-          <t>['old Codd bottle', 'Japanese Codd fruit drink bottle', 'Son', 'LittleJohn', 'MD', 'RT', 'Fascinating w']</t>
+          <t>['simple way', 'packaging', 'difference']</t>
         </is>
       </c>
       <c r="K2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2019-06-27 20:05:15</t>
+          <t>2019-06-24 18:25:26</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>RT @HollyOak4: Excited to share the latest addition to my #etsy shop: Perfume Bottle Fragrance Bottle, Avon Red Glass, Glass Bottle https:/</t>
+          <t>RT @DairiesMcqueens: How do you take your milk? With cereal? In tea or coffee? In a glass? Let us know! \n#milk #glass #glassbottle #bottle</t>
         </is>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" t="n">
-        <v>0.8706083297729492</v>
+        <v>0.8713886737823486</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -551,32 +532,35 @@
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr">
         <is>
-          <t>['Perfume Bottle Fragrance Bottle', 'Glass Bottle https', 'Avon Red Glass', 'etsy shop', 'latest addition', 'HollyOak4', 'RT']</t>
+          <t>['milk', 'glassbottle', 'RT', 'DairiesMcqueens', 'tea', 'coffee', 'cereal']</t>
         </is>
       </c>
       <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2019-06-27 19:00:10</t>
+          <t>2019-06-24 15:06:02</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>RT @HollyOak4: Excited to share the latest addition to my #etsy shop: Perfume Bottle Fragrance Bottle, Avon Red Glass, Glass Bottle https:/</t>
+          <t>Excited to share the latest addition to my #etsy shop: Organic Woodland Cologne- Men or Women Cologne, Vegan, Roll https://t.co/nLddkerTZB</t>
         </is>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0.8706083297729492</v>
+        <v>0.9230299592018127</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -592,32 +576,35 @@
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr">
         <is>
-          <t>['Perfume Bottle Fragrance Bottle', 'Glass Bottle https', 'Avon Red Glass', 'etsy shop', 'latest addition', 'HollyOak4', 'RT']</t>
+          <t>['Women Cologne', 'Organic Woodland Cologne- Men', 'etsy shop', 'latest addition', 'Vegan', 'Roll']</t>
         </is>
       </c>
       <c r="K4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2019-06-27 18:00:42</t>
+          <t>2019-06-24 11:58:03</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Shall we try this, plastic stinks bpa free or not and doesn't last long before needing replaced. #glassbottle https://t.co/zpHRbSuS2r</t>
+          <t>How do you take your milk? With cereal? In tea or coffee? In a glass? Let us know! \n#milk #glass #glassbottle https://t.co/NefHO22Gq8</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" t="n">
-        <v>0.2411497533321381</v>
+        <v>0.8751068115234375</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -633,32 +620,35 @@
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr">
         <is>
-          <t>['plastic stinks bpa free', 'glassbottle']</t>
+          <t>['milk', 'glassbottle', 'tea', 'coffee', 'cereal']</t>
         </is>
       </c>
       <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2019-06-27 16:24:37</t>
+          <t>2019-06-24 06:15:52</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>My Son brought me home a Japanese Codd fruit drink bottle. Never knew they still made the old Codd bottle. Fascinat https://t.co/zzY3GzMVb3</t>
+          <t>100ml high heel #glassbottle    #perfumeglassbottle    #uniqueperfumebottle    #specialglassperfumebottle https://t.co/VWrLEl7aoh</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>0.5</v>
+        <v>0.7552631497383118</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -674,32 +664,35 @@
       <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr">
         <is>
-          <t>['old Codd bottle', 'Japanese Codd fruit drink bottle', 'Son', 'Fascinat']</t>
+          <t>['perfumeglassbottle', 'uniqueperfumebottle', 'high heel', 'specialglassperfumebottle']</t>
         </is>
       </c>
       <c r="K6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2019-06-27 15:15:24</t>
+          <t>2019-06-24 03:55:40</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Lets make single-use a thing of the past. Stay hydrated with your Lifefactory water bottle on those hot summer day https://t.co/7tSj1m85kR</t>
+          <t>RT @chestnutcrochet: Sharing for Brenda Marsh on Etsy\n\nReally love this, from the Etsy shop PorcelainChinaArt. https://t.co/RdidXKMF6a #ets</t>
         </is>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" t="n">
-        <v>0.8530144095420837</v>
+        <v>0.5</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -715,32 +708,35 @@
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr">
         <is>
-          <t>['Lifefactory water bottle', 'hot summer day', 'thing', 'past']</t>
+          <t>['Etsy shop PorcelainChinaArt', 'love', 'Brenda Marsh', 'chestnutcrochet']</t>
         </is>
       </c>
       <c r="K7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2019-06-27 02:15:28</t>
+          <t>2019-06-23 12:39:13</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Perrier/ 750ml12 /glassbottle https://t.co/STQxKgVFIT</t>
+          <t>RT @HollyOak4: Excited to share the latest addition to my #etsy shop: Perfume Bottle Fragrance Bottle, Avon Red Glass, Glass Bottle https:/</t>
         </is>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E8" t="n">
-        <v>0.5</v>
+        <v>0.8706083297729492</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -756,32 +752,35 @@
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr">
         <is>
-          <t>['Perrier', '750ml12', 'glassbottle']</t>
+          <t>['Perfume Bottle Fragrance Bottle', 'Glass Bottle https', 'Avon Red Glass', 'etsy shop', 'latest addition', 'HollyOak4', 'RT']</t>
         </is>
       </c>
       <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2019-06-26 22:20:54</t>
+          <t>2019-06-23 11:56:00</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Excited to share the latest addition to my #etsy shop: Perfume Bottle Fragrance Bottle, Avon Red Glass, Glass Bottl https://t.co/wG5a3pb3GI</t>
+          <t>Sharing for Brenda Marsh on Etsy\n\nReally love this, from the Etsy shop PorcelainChinaArt. https://t.co/RdidXKMF6a https://t.co/CUeKOdRvGe</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E9" t="n">
-        <v>0.92364501953125</v>
+        <v>0.5</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -797,32 +796,35 @@
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr">
         <is>
-          <t>['Perfume Bottle Fragrance Bottle', 'Glass Bottl', 'Avon Red Glass', 'etsy shop', 'latest addition']</t>
+          <t>['Etsy shop PorcelainChinaArt', 'love', 'Brenda Marsh']</t>
         </is>
       </c>
       <c r="K9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2019-06-26 17:32:58</t>
+          <t>2019-06-23 04:32:45</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Wednesday Market Day!! @freiheitvillag1 3pm-7pm\nAshly will have our NEW glass spray bottles in stock.  Grab one wit https://t.co/HGy3wy8m2j</t>
+          <t>Excited to share the latest addition to my #etsy shop: Rare glass bottle by Maddock's old English lavender water https://t.co/12zdM4WpZ2</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D10" t="n">
         <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>0.5</v>
+        <v>0.8708361387252808</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -838,32 +840,35 @@
       <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr">
         <is>
-          <t>['NEW glass spray bottles', 'nAshly', 'stock', 'freiheitvillag1', 'Market Day', 'wit']</t>
+          <t>['Rare glass bottle', "Maddock's old English lavender water", 'etsy shop', 'latest addition']</t>
         </is>
       </c>
       <c r="K10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2019-06-26 14:57:54</t>
+          <t>2019-06-23 01:42:05</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Like if you are Excited! Oh Yeah\n--\n#Drink #Beer #Bottle #Label #Liqueur #Alcohol #Glassbottle #Distilledbeverage https://t.co/ZgwConGJrT</t>
+          <t>RT @HollyOak4: Excited to share the latest addition to my #etsy shop: Perfume Bottle Fragrance Bottle, Avon Red Glass, Glass Bottle https:/</t>
         </is>
       </c>
       <c r="C11" t="n">
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E11" t="n">
-        <v>0.9866830110549927</v>
+        <v>0.8706083297729492</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -879,32 +884,35 @@
       <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr">
         <is>
-          <t>['Label', 'Liqueur', 'Alcohol', 'Glassbottle', 'Beer', 'Drink', 'Distilledbeverage']</t>
+          <t>['Perfume Bottle Fragrance Bottle', 'Glass Bottle https', 'Avon Red Glass', 'etsy shop', 'latest addition', 'HollyOak4', 'RT']</t>
         </is>
       </c>
       <c r="K11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2019-06-26 02:15:28</t>
+          <t>2019-06-22 23:58:29</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Perrier/ 750ml12 /glassbottle https://t.co/STQxKgVFIT</t>
+          <t>RT @HollyOak4: Excited to share the latest addition to my #etsy shop: Perfume Bottle Fragrance Bottle, Avon Red Glass, Glass Bottle https:/</t>
         </is>
       </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E12" t="n">
-        <v>0.5</v>
+        <v>0.8706083297729492</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -920,32 +928,35 @@
       <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr">
         <is>
-          <t>['Perrier', '750ml12', 'glassbottle']</t>
+          <t>['Perfume Bottle Fragrance Bottle', 'Glass Bottle https', 'Avon Red Glass', 'etsy shop', 'latest addition', 'HollyOak4', 'RT']</t>
         </is>
       </c>
       <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2019-06-25 21:27:36</t>
+          <t>2019-06-22 20:29:08</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>RT @BagLadysCart: Eiffel Tower Replica Glass Bottle/Decanter https://t.co/M8ddyXPZo6 via @Etsy #https://www.etsy.com/shop/Gem2theiVintage #</t>
+          <t>RT @HollyOak4: Excited to share the latest addition to my #etsy shop: Perfume Bottle Fragrance Bottle, Avon Red Glass, Glass Bottle https:/</t>
         </is>
       </c>
       <c r="C13" t="n">
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E13" t="n">
-        <v>0.5</v>
+        <v>0.8706083297729492</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
@@ -961,32 +972,35 @@
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr">
         <is>
-          <t>['Eiffel Tower Replica Glass Bottle', 'Decanter', 'BagLadysCart', 'Etsy']</t>
+          <t>['Perfume Bottle Fragrance Bottle', 'Glass Bottle https', 'Avon Red Glass', 'etsy shop', 'latest addition', 'HollyOak4', 'RT']</t>
         </is>
       </c>
       <c r="K13" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2019-06-25 18:53:37</t>
+          <t>2019-06-22 19:13:39</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>RT @BagLadysCart: Eiffel Tower Replica Glass Bottle/Decanter https://t.co/M8ddyXPZo6 via @Etsy #https://www.etsy.com/shop/Gem2theiVintage #</t>
+          <t>RT @HollyOak4: Excited to share the latest addition to my #etsy shop: Perfume Bottle Fragrance Bottle, Avon Red Glass, Glass Bottle https:/</t>
         </is>
       </c>
       <c r="C14" t="n">
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E14" t="n">
-        <v>0.5</v>
+        <v>0.8706083297729492</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
@@ -1002,32 +1016,35 @@
       <c r="I14" t="inlineStr"/>
       <c r="J14" t="inlineStr">
         <is>
-          <t>['Eiffel Tower Replica Glass Bottle', 'Decanter', 'BagLadysCart', 'Etsy']</t>
+          <t>['Perfume Bottle Fragrance Bottle', 'Glass Bottle https', 'Avon Red Glass', 'etsy shop', 'latest addition', 'HollyOak4', 'RT']</t>
         </is>
       </c>
       <c r="K14" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2019-06-25 18:34:33</t>
+          <t>2019-06-22 18:42:29</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>@fitzyandwippa @MaryKayH188 @russellcrowe ...in glassbottle like https://t.co/nna7b4cchI</t>
+          <t>Excited to share the latest addition to my #etsy shop: Perfume Bottle Fragrance Bottle, Avon Red Glass, Glass Bottl https://t.co/NnpRYZBSgW</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D15" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E15" t="n">
-        <v>0.5</v>
+        <v>0.92364501953125</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -1043,29 +1060,32 @@
       <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr">
         <is>
-          <t>['MaryKayH188', 'russellcrowe', 'fitzyandwippa', 'glassbottle']</t>
+          <t>['Perfume Bottle Fragrance Bottle', 'Glass Bottl', 'Avon Red Glass', 'etsy shop', 'latest addition']</t>
         </is>
       </c>
       <c r="K15" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2019-06-25 15:29:02</t>
+          <t>2019-06-21 21:42:18</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>RT @BagLadysCart: Eiffel Tower Replica Glass Bottle/Decanter https://t.co/M8ddyXPZo6 via @Etsy #https://www.etsy.com/shop/Gem2theiVintage #</t>
+          <t>@mymilkman do you offer glass-bottle milk deliveries? Im looking for glass-bottled milk in Dublin-14 area so I can https://t.co/iqOniYhHIA</t>
         </is>
       </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E16" t="n">
         <v>0.5</v>
@@ -1084,36 +1104,39 @@
       <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr">
         <is>
-          <t>['Eiffel Tower Replica Glass Bottle', 'Decanter', 'BagLadysCart', 'Etsy']</t>
+          <t>['glass-bottled milk', 'glass-bottle milk deliveries', 'Dublin', 'area', 'Im', 'mymilkman']</t>
         </is>
       </c>
       <c r="K16" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2019-06-23 20:48:41</t>
+          <t>2019-06-24 12:39:52</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>#glass #eye... https://t.co/xhZjDFHgNt (#bottle #glassbottle #nails #eyeball #shatter #animation #animatedgif)</t>
+          <t>RT @jamesmielke: I still dont understand how #plasticbottle is intended to be a selling point for @Snapple. As if more #plastic is meant t</t>
         </is>
       </c>
       <c r="C17" t="n">
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" t="n">
-        <v>0.7720965147018433</v>
+        <v>0.167109340429306</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>glass</t>
+          <t>plastic</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -1125,36 +1148,39 @@
       <c r="I17" t="inlineStr"/>
       <c r="J17" t="inlineStr">
         <is>
-          <t>['eyeball', 'shatter', 'nails', 'animation', 'glassbottle', 'animatedgif']</t>
+          <t>['dont', 'selling point', 'RT', 'jamesmielke', 'Snapple', 'plasticbottle']</t>
         </is>
       </c>
       <c r="K17" t="n">
+        <v>0</v>
+      </c>
+      <c r="L17" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2019-06-23 12:39:13</t>
+          <t>2019-06-24 12:18:51</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>RT @HollyOak4: Excited to share the latest addition to my #etsy shop: Perfume Bottle Fragrance Bottle, Avon Red Glass, Glass Bottle https:/</t>
+          <t>I still dont understand how #plasticbottle is intended to be a selling point for @Snapple. As if more #plastic is https://t.co/RNVm8pH0QZ</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D18" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E18" t="n">
-        <v>0.8706083297729492</v>
+        <v>0.2013776302337646</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>glass</t>
+          <t>plastic</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -1166,36 +1192,39 @@
       <c r="I18" t="inlineStr"/>
       <c r="J18" t="inlineStr">
         <is>
-          <t>['Perfume Bottle Fragrance Bottle', 'Glass Bottle https', 'Avon Red Glass', 'etsy shop', 'latest addition', 'HollyOak4', 'RT']</t>
+          <t>['selling point', 'plasticbottle', 'Snapple', 'dont']</t>
         </is>
       </c>
       <c r="K18" t="n">
+        <v>0</v>
+      </c>
+      <c r="L18" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2019-06-23 11:56:00</t>
+          <t>2019-06-24 11:25:30</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Sharing for Brenda Marsh on Etsy\n\nReally love this, from the Etsy shop PorcelainChinaArt. https://t.co/RdidXKMF6a https://t.co/CUeKOdRvGe</t>
+          <t>It does not take a few seconds to throw a #PlasticBottle, but it takes a long time for it to #Decompose. \nDitch the https://t.co/o0O8kNZQnJ</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D19" t="n">
         <v>1</v>
       </c>
       <c r="E19" t="n">
-        <v>0.5</v>
+        <v>0.3036190271377563</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>glass</t>
+          <t>plastic</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -1207,36 +1236,39 @@
       <c r="I19" t="inlineStr"/>
       <c r="J19" t="inlineStr">
         <is>
-          <t>['Etsy shop PorcelainChinaArt', 'love', 'Brenda Marsh']</t>
+          <t>['PlasticBottle', 'long time', 'seconds', 'nDitch']</t>
         </is>
       </c>
       <c r="K19" t="n">
+        <v>0</v>
+      </c>
+      <c r="L19" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2019-06-23 04:32:45</t>
+          <t>2019-06-24 10:45:11</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Excited to share the latest addition to my #etsy shop: Rare glass bottle by Maddock's old English lavender water https://t.co/12zdM4WpZ2</t>
+          <t>Only a few minutes, you can make a shovel.\n#shovel #plasticbottle https://t.co/QfQBebmlYr</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D20" t="n">
         <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>0.8708361387252808</v>
+        <v>0.8193173408508301</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>glass</t>
+          <t>plastic</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -1248,22 +1280,25 @@
       <c r="I20" t="inlineStr"/>
       <c r="J20" t="inlineStr">
         <is>
-          <t>['Rare glass bottle', "Maddock's old English lavender water", 'etsy shop', 'latest addition']</t>
+          <t>['shovel', 'plasticbottle', 'minutes']</t>
         </is>
       </c>
       <c r="K20" t="n">
+        <v>0</v>
+      </c>
+      <c r="L20" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2019-06-23 02:15:28</t>
+          <t>2019-06-24 10:42:13</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Perrier/ 750ml12 /glassbottle https://t.co/STQxKgVFIT</t>
+          <t>A plastic bottle can help you separate yolks from whites.\n#plasticbottle #eggseparate https://t.co/2xMHDngRlC</t>
         </is>
       </c>
       <c r="C21" t="n">
@@ -1273,11 +1308,11 @@
         <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>0.5</v>
+        <v>0.7559324502944946</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>glass</t>
+          <t>plastic</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -1289,36 +1324,39 @@
       <c r="I21" t="inlineStr"/>
       <c r="J21" t="inlineStr">
         <is>
-          <t>['Perrier', '750ml12', 'glassbottle']</t>
+          <t>['separate yolks', 'whites', 'plasticbottle', 'plastic bottle', 'eggseparate']</t>
         </is>
       </c>
       <c r="K21" t="n">
+        <v>0</v>
+      </c>
+      <c r="L21" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2019-06-23 01:42:05</t>
+          <t>2019-06-24 10:16:23</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>RT @HollyOak4: Excited to share the latest addition to my #etsy shop: Perfume Bottle Fragrance Bottle, Avon Red Glass, Glass Bottle https:/</t>
+          <t>RT @Makerhuang1: Founded in 2006, we have over 10-year experience in producing plastic bottles. Our workshop covers an area of nearly 7,000</t>
         </is>
       </c>
       <c r="C22" t="n">
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E22" t="n">
-        <v>0.8706083297729492</v>
+        <v>0.5</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>glass</t>
+          <t>plastic</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -1330,22 +1368,25 @@
       <c r="I22" t="inlineStr"/>
       <c r="J22" t="inlineStr">
         <is>
-          <t>['Perfume Bottle Fragrance Bottle', 'Glass Bottle https', 'Avon Red Glass', 'etsy shop', 'latest addition', 'HollyOak4', 'RT']</t>
+          <t>['year experience', 'plastic bottles', 'RT', 'Makerhuang1', 'workshop', 'area']</t>
         </is>
       </c>
       <c r="K22" t="n">
+        <v>0</v>
+      </c>
+      <c r="L22" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2019-06-22 23:58:29</t>
+          <t>2019-06-24 09:35:31</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>RT @HollyOak4: Excited to share the latest addition to my #etsy shop: Perfume Bottle Fragrance Bottle, Avon Red Glass, Glass Bottle https:/</t>
+          <t>RT @RippleZoo: Because plastic lasts for so long, every single piece of #plastic ever made still exists. To put that in context, if Leonard</t>
         </is>
       </c>
       <c r="C23" t="n">
@@ -1355,11 +1396,11 @@
         <v>6</v>
       </c>
       <c r="E23" t="n">
-        <v>0.8706083297729492</v>
+        <v>0.5</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>glass</t>
+          <t>plastic</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -1371,36 +1412,39 @@
       <c r="I23" t="inlineStr"/>
       <c r="J23" t="inlineStr">
         <is>
-          <t>['Perfume Bottle Fragrance Bottle', 'Glass Bottle https', 'Avon Red Glass', 'etsy shop', 'latest addition', 'HollyOak4', 'RT']</t>
+          <t>['plastic lasts', 'RT', 'RippleZoo', 'single piece', 'context', 'Leonard']</t>
         </is>
       </c>
       <c r="K23" t="n">
+        <v>0</v>
+      </c>
+      <c r="L23" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2019-06-22 20:29:08</t>
+          <t>2019-06-24 09:16:53</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>RT @HollyOak4: Excited to share the latest addition to my #etsy shop: Perfume Bottle Fragrance Bottle, Avon Red Glass, Glass Bottle https:/</t>
+          <t>Good and natural things are always free! Refill water in your bottle do not buy!\n\n\n\n\n#plasticfree https://t.co/JzKobF7Tq1</t>
         </is>
       </c>
       <c r="C24" t="n">
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E24" t="n">
-        <v>0.8706083297729492</v>
+        <v>0.9735814332962036</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>glass</t>
+          <t>plastic</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -1412,22 +1456,25 @@
       <c r="I24" t="inlineStr"/>
       <c r="J24" t="inlineStr">
         <is>
-          <t>['Perfume Bottle Fragrance Bottle', 'Glass Bottle https', 'Avon Red Glass', 'etsy shop', 'latest addition', 'HollyOak4', 'RT']</t>
+          <t>['natural things', 'Refill water', 'bottle', 'plasticfree']</t>
         </is>
       </c>
       <c r="K24" t="n">
+        <v>0</v>
+      </c>
+      <c r="L24" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2019-06-22 19:13:39</t>
+          <t>2019-06-24 09:02:04</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>RT @HollyOak4: Excited to share the latest addition to my #etsy shop: Perfume Bottle Fragrance Bottle, Avon Red Glass, Glass Bottle https:/</t>
+          <t>RT @RippleZoo: Because plastic lasts for so long, every single piece of #plastic ever made still exists. To put that in context, if Leonard</t>
         </is>
       </c>
       <c r="C25" t="n">
@@ -1437,11 +1484,11 @@
         <v>6</v>
       </c>
       <c r="E25" t="n">
-        <v>0.8706083297729492</v>
+        <v>0.5</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>glass</t>
+          <t>plastic</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -1453,36 +1500,39 @@
       <c r="I25" t="inlineStr"/>
       <c r="J25" t="inlineStr">
         <is>
-          <t>['Perfume Bottle Fragrance Bottle', 'Glass Bottle https', 'Avon Red Glass', 'etsy shop', 'latest addition', 'HollyOak4', 'RT']</t>
+          <t>['plastic lasts', 'RT', 'RippleZoo', 'single piece', 'context', 'Leonard']</t>
         </is>
       </c>
       <c r="K25" t="n">
+        <v>0</v>
+      </c>
+      <c r="L25" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2019-06-22 18:42:29</t>
+          <t>2019-06-24 09:01:00</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Excited to share the latest addition to my #etsy shop: Perfume Bottle Fragrance Bottle, Avon Red Glass, Glass Bottl https://t.co/NnpRYZBSgW</t>
+          <t>RT @RippleZoo: Because plastic lasts for so long, every single piece of #plastic ever made still exists. To put that in context, if Leonard</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D26" t="n">
         <v>6</v>
       </c>
       <c r="E26" t="n">
-        <v>0.92364501953125</v>
+        <v>0.5</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>glass</t>
+          <t>plastic</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -1494,36 +1544,39 @@
       <c r="I26" t="inlineStr"/>
       <c r="J26" t="inlineStr">
         <is>
-          <t>['Perfume Bottle Fragrance Bottle', 'Glass Bottl', 'Avon Red Glass', 'etsy shop', 'latest addition']</t>
+          <t>['plastic lasts', 'RT', 'RippleZoo', 'single piece', 'context', 'Leonard']</t>
         </is>
       </c>
       <c r="K26" t="n">
+        <v>0</v>
+      </c>
+      <c r="L26" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2019-06-22 02:15:28</t>
+          <t>2019-06-24 09:00:24</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Perrier/ 750ml12 /glassbottle https://t.co/STQxKgVFIT</t>
+          <t>Because plastic lasts for so long, every single piece of #plastic ever made still exists. To put that in context, i https://t.co/9UemeBFsKu</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="D27" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E27" t="n">
-        <v>0.5</v>
+        <v>0.2493803203105927</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>glass</t>
+          <t>plastic</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
@@ -1535,36 +1588,39 @@
       <c r="I27" t="inlineStr"/>
       <c r="J27" t="inlineStr">
         <is>
-          <t>['Perrier', '750ml12', 'glassbottle']</t>
+          <t>['plastic lasts', 'single piece', 'context']</t>
         </is>
       </c>
       <c r="K27" t="n">
+        <v>0</v>
+      </c>
+      <c r="L27" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2019-06-21 21:42:18</t>
+          <t>2019-06-24 03:51:36</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>@mymilkman do you offer glass-bottle milk deliveries? Im looking for glass-bottled milk in Dublin-14 area so I can https://t.co/iqOniYhHIA</t>
+          <t>Founded in 2006, we have over 10-year experience in producing plastic bottles. Our workshop covers an area of nearl https://t.co/8fFzVNmXVq</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D28" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E28" t="n">
-        <v>0.5</v>
+        <v>0.685232400894165</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>glass</t>
+          <t>plastic</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
@@ -1576,22 +1632,25 @@
       <c r="I28" t="inlineStr"/>
       <c r="J28" t="inlineStr">
         <is>
-          <t>['glass-bottled milk', 'glass-bottle milk deliveries', 'Dublin', 'area', 'Im', 'mymilkman']</t>
+          <t>['year experience', 'plastic bottles', 'workshop', 'area of nearl']</t>
         </is>
       </c>
       <c r="K28" t="n">
+        <v>0</v>
+      </c>
+      <c r="L28" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2019-06-21 13:14:42</t>
+          <t>2019-06-23 05:56:20</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Glass object of antique glass, archeological findings, glass art work https://t.co/Ti36FB5bOy #art #mixedmedia https://t.co/BbocyxiyHQ</t>
+          <t>@engineers_feed And according to this gov study in #Austria where the #plasticbottle is from, only 28% are recycled https://t.co/sFWLOq0imZ</t>
         </is>
       </c>
       <c r="C29" t="n">
@@ -1601,11 +1660,11 @@
         <v>0</v>
       </c>
       <c r="E29" t="n">
-        <v>0.2612619996070862</v>
+        <v>0.2456267774105072</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>glass</t>
+          <t>plastic</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
@@ -1617,22 +1676,25 @@
       <c r="I29" t="inlineStr"/>
       <c r="J29" t="inlineStr">
         <is>
-          <t>['Glass object of antique glass', 'glass art work', 'archeological findings', 'mixedmedia']</t>
+          <t>['feed', 'Austria', 'gov study', 'plasticbottle', 'engineers']</t>
         </is>
       </c>
       <c r="K29" t="n">
+        <v>0</v>
+      </c>
+      <c r="L29" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2019-06-21 07:55:49</t>
+          <t>2019-06-23 02:37:05</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>PLASTIC  how is it #activistposter #drawings #plastic #fuckdoll #activist #streetartactivist #plasticfree https://t.co/tBJAFiv2R0</t>
+          <t>#aqua #product #drinkware #glass #plasticbottle #bottle #water #plastic #turquoise\n\nFREE Shipping Worldwide\nGet it https://t.co/vtTG3L9do0</t>
         </is>
       </c>
       <c r="C30" t="n">
@@ -1642,11 +1704,11 @@
         <v>0</v>
       </c>
       <c r="E30" t="n">
-        <v>0.7941458225250244</v>
+        <v>0.5</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>glass</t>
+          <t>plastic</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
@@ -1658,36 +1720,39 @@
       <c r="I30" t="inlineStr"/>
       <c r="J30" t="inlineStr">
         <is>
-          <t>['fuckdoll', 'streetartactivist', 'drawings', 'activistposter', 'plasticfree']</t>
+          <t>['glass', 'water', 'plasticbottle', 'drinkware', 'Shipping', 'product', 'nGet']</t>
         </is>
       </c>
       <c r="K30" t="n">
+        <v>0</v>
+      </c>
+      <c r="L30" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2019-06-21 05:50:30</t>
+          <t>2019-06-22 01:06:25</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>RT @Harmeen: #Recycled #DecoupagedGlassBottle \nIt's fun turning #trashinto #TREASURE \n#recycling #glassbottle into a #vase    #inexpensive</t>
+          <t>RT @LeoWolfy: When an artist finishes your commission https://t.co/GdNYGQ4PvL</t>
         </is>
       </c>
       <c r="C31" t="n">
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>1</v>
+        <v>35308</v>
       </c>
       <c r="E31" t="n">
-        <v>0.8239593505859375</v>
+        <v>0.5</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>glass</t>
+          <t>plastic</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
@@ -1699,36 +1764,39 @@
       <c r="I31" t="inlineStr"/>
       <c r="J31" t="inlineStr">
         <is>
-          <t>['trashinto', 'TREASURE', 'recycling', 'DecoupagedGlassBottle', "nIt's fun", 'vase', 'Harmeen', 'RT']</t>
+          <t>['artist', 'LeoWolfy', 'commission']</t>
         </is>
       </c>
       <c r="K31" t="n">
+        <v>0</v>
+      </c>
+      <c r="L31" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2019-06-26 17:39:31</t>
+          <t>2019-06-24 17:54:56</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>RT @deeperblue: T\nMade using natural rubber and recycled plastic bottles, Rock Hopper dive shoes are good for your feet AND good for the oc</t>
+          <t>Excited to share the latest addition to my #etsy shop: Vintage Glass and metal sugar pour container, 1990s, Kitchen https://t.co/ZeGV7vrvAj</t>
         </is>
       </c>
       <c r="C32" t="n">
         <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E32" t="n">
-        <v>0.9193069338798523</v>
+        <v>0.8440326452255249</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>plastic</t>
+          <t>glass</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
@@ -1740,32 +1808,35 @@
       <c r="I32" t="inlineStr"/>
       <c r="J32" t="inlineStr">
         <is>
-          <t>['recycled plastic bottles', 'Rock Hopper dive shoes', 'nMade', 'natural rubber', 'feet', 'deeperblue', 'RT']</t>
+          <t>['etsy shop', 'metal sugar', 'container', 'Vintage Glass', 'latest addition', 'Kitchen']</t>
         </is>
       </c>
       <c r="K32" t="n">
+        <v>0</v>
+      </c>
+      <c r="L32" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2019-06-26 17:19:12</t>
+          <t>2019-06-24 21:01:03</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>RT @deeperblue: T\nMade using natural rubber and recycled plastic bottles, Rock Hopper dive shoes are good for your feet AND good for the oc</t>
+          <t>Rounded corners and smooth surfaces better protects produce, increasing the yield of your harvest!\n\n#harvestbin https://t.co/Wak0Ca5zKr</t>
         </is>
       </c>
       <c r="C33" t="n">
         <v>0</v>
       </c>
       <c r="D33" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E33" t="n">
-        <v>0.9193069338798523</v>
+        <v>0.8738755583763123</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
@@ -1781,543 +1852,13 @@
       <c r="I33" t="inlineStr"/>
       <c r="J33" t="inlineStr">
         <is>
-          <t>['recycled plastic bottles', 'Rock Hopper dive shoes', 'nMade', 'natural rubber', 'feet', 'deeperblue', 'RT']</t>
+          <t>['produce', 'smooth surfaces', 'Rounded corners', 'yield', 'harvestbin']</t>
         </is>
       </c>
       <c r="K33" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>2019-06-26 17:00:35</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>T\nMade using natural rubber and recycled plastic bottles, Rock Hopper dive shoes are good for your feet AND good fo https://t.co/w0TFNcwPN9</t>
-        </is>
-      </c>
-      <c r="C34" t="n">
-        <v>2</v>
-      </c>
-      <c r="D34" t="n">
-        <v>2</v>
-      </c>
-      <c r="E34" t="n">
-        <v>0.9258869886398315</v>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>plastic</t>
-        </is>
-      </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>Product</t>
-        </is>
-      </c>
-      <c r="H34" t="inlineStr"/>
-      <c r="I34" t="inlineStr"/>
-      <c r="J34" t="inlineStr">
-        <is>
-          <t>['good fo', 'recycled plastic bottles', 'Rock Hopper dive shoes', 'natural rubber', 'nMade', 'feet']</t>
-        </is>
-      </c>
-      <c r="K34" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>2019-06-25 20:40:35</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>RT @RippleZoo: Because plastic lasts for so long, every single piece of #plastic ever made still exists. To put that in context, if Leonard</t>
-        </is>
-      </c>
-      <c r="C35" t="n">
-        <v>0</v>
-      </c>
-      <c r="D35" t="n">
-        <v>6</v>
-      </c>
-      <c r="E35" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>plastic</t>
-        </is>
-      </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>Product</t>
-        </is>
-      </c>
-      <c r="H35" t="inlineStr"/>
-      <c r="I35" t="inlineStr"/>
-      <c r="J35" t="inlineStr">
-        <is>
-          <t>['plastic lasts', 'RT', 'RippleZoo', 'single piece', 'context', 'Leonard']</t>
-        </is>
-      </c>
-      <c r="K35" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>2019-06-25 14:18:51</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>DIY/Waste #Plasticbottle #FlowerVase New Ideas #WoolenGuldasta https://t.co/1J1SPkJSGU via @YouTube</t>
-        </is>
-      </c>
-      <c r="C36" t="n">
-        <v>2</v>
-      </c>
-      <c r="D36" t="n">
-        <v>0</v>
-      </c>
-      <c r="E36" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>plastic</t>
-        </is>
-      </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>Product</t>
-        </is>
-      </c>
-      <c r="H36" t="inlineStr"/>
-      <c r="I36" t="inlineStr"/>
-      <c r="J36" t="inlineStr">
-        <is>
-          <t>['Plasticbottle', 'FlowerVase New Ideas', 'WoolenGuldasta', 'Waste', 'DIY', 'YouTube']</t>
-        </is>
-      </c>
-      <c r="K36" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>2019-06-25 09:19:57</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>Unusual #plasticbottle design of Zabava sunflower oil https://t.co/dcBnjE494R #packaging https://t.co/BsqK1HRkP0</t>
-        </is>
-      </c>
-      <c r="C37" t="n">
-        <v>0</v>
-      </c>
-      <c r="D37" t="n">
-        <v>0</v>
-      </c>
-      <c r="E37" t="n">
-        <v>0.7688534259796143</v>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>plastic</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>Product</t>
-        </is>
-      </c>
-      <c r="H37" t="inlineStr"/>
-      <c r="I37" t="inlineStr"/>
-      <c r="J37" t="inlineStr">
-        <is>
-          <t>['plasticbottle design of Zabava sunflower oil', 'packaging']</t>
-        </is>
-      </c>
-      <c r="K37" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>2019-06-25 06:34:19</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>Hulls Industry body water refill stations to reduce plastics bottles a splash hit.\nRead More - https://t.co/1rVQt1WLYm</t>
-        </is>
-      </c>
-      <c r="C38" t="n">
-        <v>1</v>
-      </c>
-      <c r="D38" t="n">
-        <v>0</v>
-      </c>
-      <c r="E38" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>plastic</t>
-        </is>
-      </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>Product</t>
-        </is>
-      </c>
-      <c r="H38" t="inlineStr"/>
-      <c r="I38" t="inlineStr"/>
-      <c r="J38" t="inlineStr">
-        <is>
-          <t>['plastics', 'Hulls Industry body water refill stations', 'splash hit', 'nRead']</t>
-        </is>
-      </c>
-      <c r="K38" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>2019-06-24 12:39:52</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>RT @jamesmielke: I still dont understand how #plasticbottle is intended to be a selling point for @Snapple. As if more #plastic is meant t</t>
-        </is>
-      </c>
-      <c r="C39" t="n">
-        <v>0</v>
-      </c>
-      <c r="D39" t="n">
-        <v>1</v>
-      </c>
-      <c r="E39" t="n">
-        <v>0.167109340429306</v>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>plastic</t>
-        </is>
-      </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>Product</t>
-        </is>
-      </c>
-      <c r="H39" t="inlineStr"/>
-      <c r="I39" t="inlineStr"/>
-      <c r="J39" t="inlineStr">
-        <is>
-          <t>['dont', 'selling point', 'RT', 'jamesmielke', 'Snapple', 'plasticbottle']</t>
-        </is>
-      </c>
-      <c r="K39" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>2019-06-24 12:18:51</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>I still dont understand how #plasticbottle is intended to be a selling point for @Snapple. As if more #plastic is https://t.co/RNVm8pH0QZ</t>
-        </is>
-      </c>
-      <c r="C40" t="n">
-        <v>4</v>
-      </c>
-      <c r="D40" t="n">
-        <v>1</v>
-      </c>
-      <c r="E40" t="n">
-        <v>0.2013776302337646</v>
-      </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>plastic</t>
-        </is>
-      </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t>Product</t>
-        </is>
-      </c>
-      <c r="H40" t="inlineStr"/>
-      <c r="I40" t="inlineStr"/>
-      <c r="J40" t="inlineStr">
-        <is>
-          <t>['selling point', 'plasticbottle', 'Snapple', 'dont']</t>
-        </is>
-      </c>
-      <c r="K40" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>2019-06-24 11:29:03</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>RT @cabanamic: me di cuenta que siempre termino hablando de mi onda por ah me estas contando no s que se muri tu abuela y yo voy a poner</t>
-        </is>
-      </c>
-      <c r="C41" t="n">
-        <v>0</v>
-      </c>
-      <c r="D41" t="n">
-        <v>10538</v>
-      </c>
-      <c r="E41" t="n">
-        <v>0.7012739181518555</v>
-      </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>plastic</t>
-        </is>
-      </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>Product</t>
-        </is>
-      </c>
-      <c r="H41" t="inlineStr"/>
-      <c r="I41" t="inlineStr"/>
-      <c r="J41" t="inlineStr">
-        <is>
-          <t>['cuenta que siempre termino hablando', 's que se muri tu abuela y yo voy', 'estas contando', 'mi onda por ah', 'poner', 'cabanamic', 'RT']</t>
-        </is>
-      </c>
-      <c r="K41" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>2019-06-24 11:25:30</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>It does not take a few seconds to throw a #PlasticBottle, but it takes a long time for it to #Decompose. \nDitch the https://t.co/o0O8kNZQnJ</t>
-        </is>
-      </c>
-      <c r="C42" t="n">
-        <v>5</v>
-      </c>
-      <c r="D42" t="n">
-        <v>1</v>
-      </c>
-      <c r="E42" t="n">
-        <v>0.3036190271377563</v>
-      </c>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>plastic</t>
-        </is>
-      </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>Product</t>
-        </is>
-      </c>
-      <c r="H42" t="inlineStr"/>
-      <c r="I42" t="inlineStr"/>
-      <c r="J42" t="inlineStr">
-        <is>
-          <t>['PlasticBottle', 'long time', 'seconds', 'nDitch']</t>
-        </is>
-      </c>
-      <c r="K42" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>2019-06-24 10:45:11</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>Only a few minutes, you can make a shovel.\n#shovel #plasticbottle https://t.co/QfQBebmlYr</t>
-        </is>
-      </c>
-      <c r="C43" t="n">
-        <v>0</v>
-      </c>
-      <c r="D43" t="n">
-        <v>0</v>
-      </c>
-      <c r="E43" t="n">
-        <v>0.8193173408508301</v>
-      </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>plastic</t>
-        </is>
-      </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>Product</t>
-        </is>
-      </c>
-      <c r="H43" t="inlineStr"/>
-      <c r="I43" t="inlineStr"/>
-      <c r="J43" t="inlineStr">
-        <is>
-          <t>['shovel', 'plasticbottle', 'minutes']</t>
-        </is>
-      </c>
-      <c r="K43" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>2019-06-24 10:42:13</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>A plastic bottle can help you separate yolks from whites.\n#plasticbottle #eggseparate https://t.co/2xMHDngRlC</t>
-        </is>
-      </c>
-      <c r="C44" t="n">
-        <v>0</v>
-      </c>
-      <c r="D44" t="n">
-        <v>0</v>
-      </c>
-      <c r="E44" t="n">
-        <v>0.7559324502944946</v>
-      </c>
-      <c r="F44" t="inlineStr">
-        <is>
-          <t>plastic</t>
-        </is>
-      </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>Product</t>
-        </is>
-      </c>
-      <c r="H44" t="inlineStr"/>
-      <c r="I44" t="inlineStr"/>
-      <c r="J44" t="inlineStr">
-        <is>
-          <t>['separate yolks', 'whites', 'plasticbottle', 'plastic bottle', 'eggseparate']</t>
-        </is>
-      </c>
-      <c r="K44" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>2019-06-24 10:16:23</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>RT @Makerhuang1: Founded in 2006, we have over 10-year experience in producing plastic bottles. Our workshop covers an area of nearly 7,000</t>
-        </is>
-      </c>
-      <c r="C45" t="n">
-        <v>0</v>
-      </c>
-      <c r="D45" t="n">
-        <v>2</v>
-      </c>
-      <c r="E45" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t>plastic</t>
-        </is>
-      </c>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>Product</t>
-        </is>
-      </c>
-      <c r="H45" t="inlineStr"/>
-      <c r="I45" t="inlineStr"/>
-      <c r="J45" t="inlineStr">
-        <is>
-          <t>['year experience', 'plastic bottles', 'RT', 'Makerhuang1', 'workshop', 'area']</t>
-        </is>
-      </c>
-      <c r="K45" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>2019-06-24 09:35:31</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>RT @RippleZoo: Because plastic lasts for so long, every single piece of #plastic ever made still exists. To put that in context, if Leonard</t>
-        </is>
-      </c>
-      <c r="C46" t="n">
-        <v>0</v>
-      </c>
-      <c r="D46" t="n">
-        <v>6</v>
-      </c>
-      <c r="E46" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>plastic</t>
-        </is>
-      </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>Product</t>
-        </is>
-      </c>
-      <c r="H46" t="inlineStr"/>
-      <c r="I46" t="inlineStr"/>
-      <c r="J46" t="inlineStr">
-        <is>
-          <t>['plastic lasts', 'RT', 'RippleZoo', 'single piece', 'context', 'Leonard']</t>
-        </is>
-      </c>
-      <c r="K46" t="n">
+      <c r="L33" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2332,13 +1873,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
@@ -2353,7 +1894,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Lifestyle</t>
+          <t>Cost</t>
         </is>
       </c>
     </row>
@@ -2363,7 +1904,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Cost</t>
+          <t>Aesthetic</t>
         </is>
       </c>
     </row>
@@ -2373,7 +1914,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Aesthetic</t>
+          <t>Product</t>
         </is>
       </c>
     </row>
@@ -2383,7 +1924,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Product</t>
+          <t>Sustainability</t>
         </is>
       </c>
     </row>
@@ -2393,7 +1934,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Sustainability</t>
+          <t>Art</t>
         </is>
       </c>
     </row>
@@ -2403,7 +1944,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Art</t>
+          <t>Convenience</t>
         </is>
       </c>
     </row>
@@ -2413,7 +1954,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Convenience</t>
+          <t>Innovation</t>
         </is>
       </c>
     </row>
@@ -2422,16 +1963,6 @@
         <v>7</v>
       </c>
       <c r="B9" t="inlineStr">
-        <is>
-          <t>Innovation</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="inlineStr">
         <is>
           <t>Advertisement</t>
         </is>

</xml_diff>